<commit_message>
Update Abnormalities_Features - V2.xlsx
</commit_message>
<xml_diff>
--- a/Toy-example/Abnormalities_Features - V2.xlsx
+++ b/Toy-example/Abnormalities_Features - V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp zbook g5\Documents\GitHub\paper-TDA-embankment-monitoring\Toy-example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBEB554A-0F28-45CD-9129-738DAC134C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57E15F4-FA72-48BC-B47F-EC62EB23E3F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F2A9B525-589D-4D02-9202-6C3488D882EF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>PE (H0)</t>
   </si>
@@ -85,6 +85,12 @@
   <si>
     <t>Heat amp (H1)</t>
   </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
 </sst>
 </file>
 
@@ -113,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -125,12 +131,62 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -141,14 +197,12 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right/>
@@ -161,12 +215,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -176,27 +226,14 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -205,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,32 +250,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8641D189-C2AF-41F1-9692-F40E39958ABB}">
-  <dimension ref="B2:R22"/>
+  <dimension ref="B3:R23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="B3:C22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,1066 +645,1090 @@
     <col min="24" max="24" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B3" s="11"/>
-      <c r="C3" s="2" t="s">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="C3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="14"/>
+    </row>
+    <row r="4" spans="2:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="3" t="s">
+      <c r="Q4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="R4" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
         <v>-50</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C5" s="3">
         <v>11.4</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5" s="4">
         <v>8.93</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E5" s="4">
         <v>3000</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F5" s="4">
         <v>793</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G5" s="4">
         <v>3.41</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H5" s="4">
         <v>4.6100000000000003</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I5" s="4">
         <v>76.2</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J5" s="4">
         <v>27.8</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K5" s="4">
         <v>5.14</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L5" s="4">
         <v>8.56</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M5" s="4">
         <v>2210</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N5" s="4">
         <v>235</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O5" s="4">
         <v>4160</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P5" s="4">
         <v>453</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q5" s="4">
         <v>2900</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R5" s="4">
         <v>304</v>
       </c>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="5">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
         <v>-40</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C6" s="3">
         <v>11.3875660990109</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="4">
         <v>8.8984492732473903</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E6" s="4">
         <v>2999</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F6" s="4">
         <v>778</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G6" s="4">
         <v>3.5741289854049598</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H6" s="4">
         <v>4.1962463855743399</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I6" s="4">
         <v>76.000984169053098</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J6" s="4">
         <v>27.2246865266697</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K6" s="4">
         <v>5.5168421697891201</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L6" s="4">
         <v>7.8818827212961402</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M6" s="4">
         <v>2176.09415439128</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N6" s="4">
         <v>219.32192025017301</v>
       </c>
-      <c r="O5" s="7">
+      <c r="O6" s="4">
         <v>4121.9914644221599</v>
       </c>
-      <c r="P5" s="7">
+      <c r="P6" s="4">
         <v>437.43666896753899</v>
       </c>
-      <c r="Q5" s="7">
+      <c r="Q6" s="4">
         <v>2902.97284038404</v>
       </c>
-      <c r="R5" s="7">
+      <c r="R6" s="4">
         <v>289.27207466694898</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
         <v>-30</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C7" s="3">
         <v>11.4</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="4">
         <v>8.92</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E7" s="4">
         <v>3000</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F7" s="4">
         <v>786</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G7" s="4">
         <v>3.51</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H7" s="4">
         <v>4.32</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I7" s="4">
         <v>76.2</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J7" s="4">
         <v>27.1</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K7" s="4">
         <v>5.38</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L7" s="4">
         <v>7.96</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M7" s="4">
         <v>2180</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N7" s="4">
         <v>224</v>
       </c>
-      <c r="O6" s="7">
+      <c r="O7" s="4">
         <v>4130</v>
       </c>
-      <c r="P6" s="7">
+      <c r="P7" s="4">
         <v>441</v>
       </c>
-      <c r="Q6" s="7">
+      <c r="Q7" s="4">
         <v>2900</v>
       </c>
-      <c r="R6" s="7">
+      <c r="R7" s="4">
         <v>292</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="5">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
         <v>-20</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C8" s="3">
         <v>11.397983125542501</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D8" s="4">
         <v>8.93586340862527</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E8" s="4">
         <v>2999</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F8" s="4">
         <v>798</v>
       </c>
-      <c r="G7" s="7">
+      <c r="G8" s="4">
         <v>3.6679002046584999</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H8" s="4">
         <v>4.2695848941802899</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I8" s="4">
         <v>76.144269874762699</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J8" s="4">
         <v>27.399616505947101</v>
       </c>
-      <c r="K7" s="7">
+      <c r="K8" s="4">
         <v>5.7354493314181099</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L8" s="4">
         <v>7.7951187588912196</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M8" s="4">
         <v>2202.9499935516101</v>
       </c>
-      <c r="N7" s="7">
+      <c r="N8" s="4">
         <v>231.20028630465299</v>
       </c>
-      <c r="O7" s="7">
+      <c r="O8" s="4">
         <v>4165.40855966454</v>
       </c>
-      <c r="P7" s="7">
+      <c r="P8" s="4">
         <v>445.61501498844302</v>
       </c>
-      <c r="Q7" s="7">
+      <c r="Q8" s="4">
         <v>2954.67352588936</v>
       </c>
-      <c r="R7" s="7">
+      <c r="R8" s="4">
         <v>299.71983821977398</v>
       </c>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B8" s="5">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B9" s="2">
         <v>-15</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C9" s="3">
         <v>11.4</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D9" s="4">
         <v>8.9600000000000009</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E9" s="4">
         <v>3000</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F9" s="4">
         <v>794</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G9" s="4">
         <v>3.53</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H9" s="4">
         <v>4.1100000000000003</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I9" s="4">
         <v>76.599999999999994</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J9" s="4">
         <v>27.4</v>
       </c>
-      <c r="K8" s="7">
+      <c r="K9" s="4">
         <v>5.41</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L9" s="4">
         <v>7.67</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M9" s="4">
         <v>2190</v>
       </c>
-      <c r="N8" s="7">
+      <c r="N9" s="4">
         <v>230</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O9" s="4">
         <v>4150</v>
       </c>
-      <c r="P8" s="7">
+      <c r="P9" s="4">
         <v>459</v>
       </c>
-      <c r="Q8" s="7">
+      <c r="Q9" s="4">
         <v>2890</v>
       </c>
-      <c r="R8" s="7">
+      <c r="R9" s="4">
         <v>301</v>
       </c>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B9" s="5">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
         <v>-10</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C10" s="3">
         <v>11.4</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D10" s="4">
         <v>8.9499999999999993</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E10" s="4">
         <v>3000</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F10" s="4">
         <v>788</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G10" s="4">
         <v>3.88</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H10" s="4">
         <v>4.1500000000000004</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I10" s="4">
         <v>76.099999999999994</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J10" s="4">
         <v>27</v>
       </c>
-      <c r="K9" s="7">
+      <c r="K10" s="4">
         <v>6.23</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L10" s="4">
         <v>7.48</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M10" s="4">
         <v>2210</v>
       </c>
-      <c r="N9" s="7">
+      <c r="N10" s="4">
         <v>227</v>
       </c>
-      <c r="O9" s="7">
+      <c r="O10" s="4">
         <v>4160</v>
       </c>
-      <c r="P9" s="7">
+      <c r="P10" s="4">
         <v>444</v>
       </c>
-      <c r="Q9" s="7">
+      <c r="Q10" s="4">
         <v>2950</v>
       </c>
-      <c r="R9" s="7">
+      <c r="R10" s="4">
         <v>294</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="5">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
         <v>-7</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C11" s="3">
         <v>11.4</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D11" s="4">
         <v>8.94</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E11" s="4">
         <v>3000</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F11" s="4">
         <v>801</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G11" s="4">
         <v>3.6</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H11" s="4">
         <v>4.37</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I11" s="4">
         <v>76</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J11" s="4">
         <v>26.9</v>
       </c>
-      <c r="K10" s="7">
+      <c r="K11" s="4">
         <v>5.57</v>
       </c>
-      <c r="L10" s="7">
+      <c r="L11" s="4">
         <v>8.0500000000000007</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M11" s="4">
         <v>2190</v>
       </c>
-      <c r="N10" s="7">
+      <c r="N11" s="4">
         <v>235</v>
       </c>
-      <c r="O10" s="7">
+      <c r="O11" s="4">
         <v>4140</v>
       </c>
-      <c r="P10" s="7">
+      <c r="P11" s="4">
         <v>444</v>
       </c>
-      <c r="Q10" s="7">
+      <c r="Q11" s="4">
         <v>2900</v>
       </c>
-      <c r="R10" s="7">
+      <c r="R11" s="4">
         <v>297</v>
       </c>
     </row>
-    <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="5">
+    <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="2">
         <v>-4</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C12" s="3">
         <v>11.397219133262899</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D12" s="4">
         <v>8.9604588940337102</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E12" s="4">
         <v>2999</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F12" s="4">
         <v>810.5</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G12" s="4">
         <v>3.3463776111602699</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H12" s="4">
         <v>4.2982076406478802</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I12" s="4">
         <v>76.698959619038007</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J12" s="4">
         <v>27.159008963184</v>
       </c>
-      <c r="K11" s="7">
+      <c r="K12" s="4">
         <v>4.9980762123429097</v>
       </c>
-      <c r="L11" s="7">
+      <c r="L12" s="4">
         <v>7.9705773226732397</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M12" s="4">
         <v>2196.5875836915502</v>
       </c>
-      <c r="N11" s="7">
+      <c r="N12" s="4">
         <v>243.49367164360899</v>
       </c>
-      <c r="O11" s="7">
+      <c r="O12" s="4">
         <v>4175.1823474123603</v>
       </c>
-      <c r="P11" s="7">
+      <c r="P12" s="4">
         <v>452.55886019168901</v>
       </c>
-      <c r="Q11" s="7">
+      <c r="Q12" s="4">
         <v>2904.4473869650501</v>
       </c>
-      <c r="R11" s="7">
+      <c r="R12" s="4">
         <v>311.21458636275702</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="8">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B13" s="5">
         <v>-2</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C13" s="3">
         <v>11.395678953057899</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D13" s="4">
         <v>8.9342694789378498</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E13" s="4">
         <v>2999</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F13" s="4">
         <v>792.5</v>
       </c>
-      <c r="G12" s="7">
+      <c r="G13" s="4">
         <v>3.8268494606018</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H13" s="4">
         <v>4.4640449285507202</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I13" s="4">
         <v>76.237979614162498</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J13" s="4">
         <v>27.666424607861199</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K13" s="4">
         <v>6.1144648036175102</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L13" s="4">
         <v>8.4710957559181796</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M13" s="4">
         <v>2196.6591463641598</v>
       </c>
-      <c r="N12" s="7">
+      <c r="N13" s="4">
         <v>227.762408646593</v>
       </c>
-      <c r="O12" s="7">
+      <c r="O13" s="4">
         <v>4164.4183421510697</v>
       </c>
-      <c r="P12" s="7">
+      <c r="P13" s="4">
         <v>443.81504294276601</v>
       </c>
-      <c r="Q12" s="7">
+      <c r="Q13" s="4">
         <v>2965.92195826951</v>
       </c>
-      <c r="R12" s="7">
+      <c r="R13" s="4">
         <v>298.02962204643001</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
+    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B14" s="6">
         <v>0</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C14" s="3">
         <v>11.3889410503359</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D14" s="4">
         <v>8.9598497340314491</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E14" s="4">
         <v>2999</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F14" s="4">
         <v>798</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G14" s="4">
         <v>3.5099474191665601</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H14" s="4">
         <v>3.7904499769210802</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I14" s="4">
         <v>76.426591351301099</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J14" s="4">
         <v>27.249006080617001</v>
       </c>
-      <c r="K13" s="7">
+      <c r="K14" s="4">
         <v>5.3693152973797602</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L14" s="4">
         <v>7.2349792057106104</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M14" s="4">
         <v>2170.5903256696001</v>
       </c>
-      <c r="N13" s="7">
+      <c r="N14" s="4">
         <v>234.71276632601101</v>
       </c>
-      <c r="O13" s="7">
+      <c r="O14" s="4">
         <v>4143.0847656014203</v>
       </c>
-      <c r="P13" s="7">
+      <c r="P14" s="4">
         <v>458.27932286775501</v>
       </c>
-      <c r="Q13" s="7">
+      <c r="Q14" s="4">
         <v>2897.0450953332902</v>
       </c>
-      <c r="R13" s="7">
+      <c r="R14" s="4">
         <v>304.14791541108701</v>
       </c>
     </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B14" s="5">
+    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C15" s="3">
         <v>11.3848693367768</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D15" s="4">
         <v>8.9069798721178604</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E15" s="4">
         <v>2999</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F15" s="4">
         <v>776.5</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G15" s="4">
         <v>3.3882874250411898</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H15" s="4">
         <v>3.94506764411926</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I15" s="4">
         <v>75.883958257424993</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J15" s="4">
         <v>27.708693400301499</v>
       </c>
-      <c r="K14" s="7">
+      <c r="K15" s="4">
         <v>5.0922005292985997</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L15" s="4">
         <v>7.4222626844565101</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M15" s="4">
         <v>2157.9971148630402</v>
       </c>
-      <c r="N14" s="7">
+      <c r="N15" s="4">
         <v>223.520221085006</v>
       </c>
-      <c r="O14" s="7">
+      <c r="O15" s="4">
         <v>4117.9366044850603</v>
       </c>
-      <c r="P14" s="7">
+      <c r="P15" s="4">
         <v>443.92693426561902</v>
       </c>
-      <c r="Q14" s="7">
+      <c r="Q15" s="4">
         <v>2869.0942537299202</v>
       </c>
-      <c r="R14" s="7">
+      <c r="R15" s="4">
         <v>290.90833687382298</v>
       </c>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="5">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B16" s="2">
         <v>4</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C16" s="3">
         <v>11.3936572585608</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D16" s="4">
         <v>8.9384835095310304</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E16" s="4">
         <v>2999</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F16" s="4">
         <v>783.5</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G16" s="4">
         <v>3.6082196235656698</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H16" s="4">
         <v>4.0427705049514699</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I16" s="4">
         <v>76.118204619644203</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J16" s="4">
         <v>27.120398375090002</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K16" s="4">
         <v>5.5959927527686197</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L16" s="4">
         <v>7.4641760063291898</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M16" s="4">
         <v>2199.6429536258202</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N16" s="4">
         <v>225.28571329135701</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O16" s="4">
         <v>4154.4297028139299</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P16" s="4">
         <v>447.22847062974398</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q16" s="4">
         <v>2915.8402487012399</v>
       </c>
-      <c r="R15" s="7">
+      <c r="R16" s="4">
         <v>294.14966532685901</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="5">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B17" s="2">
         <v>7</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C17" s="3">
         <v>11.391465966431699</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D17" s="4">
         <v>8.9736481316910197</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E17" s="4">
         <v>2999</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F17" s="4">
         <v>810.5</v>
       </c>
-      <c r="G16" s="7">
+      <c r="G17" s="4">
         <v>4.1009571552276602</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H17" s="4">
         <v>4.1587321758270201</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I17" s="4">
         <v>76.692291614412099</v>
       </c>
-      <c r="J16" s="7">
+      <c r="J17" s="4">
         <v>26.787134661924799</v>
       </c>
-      <c r="K16" s="7">
+      <c r="K17" s="4">
         <v>6.7809683531045</v>
       </c>
-      <c r="L16" s="7">
+      <c r="L17" s="4">
         <v>7.6613569767321898</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M17" s="4">
         <v>2189.0638999684002</v>
       </c>
-      <c r="N16" s="7">
+      <c r="N17" s="4">
         <v>236.24476054659999</v>
       </c>
-      <c r="O16" s="7">
+      <c r="O17" s="4">
         <v>4162.7497686377901</v>
       </c>
-      <c r="P16" s="7">
+      <c r="P17" s="4">
         <v>453.00040754435298</v>
       </c>
-      <c r="Q16" s="7">
+      <c r="Q17" s="4">
         <v>2970.82807284416</v>
       </c>
-      <c r="R16" s="7">
+      <c r="R17" s="4">
         <v>307.17947602683302</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="5">
+    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B18" s="2">
         <v>10</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C18" s="3">
         <v>11.390773272870099</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D18" s="4">
         <v>8.9420324575590495</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E18" s="4">
         <v>2999</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F18" s="4">
         <v>791</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G18" s="4">
         <v>3.5306950807571398</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H18" s="4">
         <v>3.9610126018524099</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I18" s="4">
         <v>76.276793154377003</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J18" s="4">
         <v>27.983603134557899</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K18" s="4">
         <v>5.4165472275040001</v>
       </c>
-      <c r="L17" s="7">
+      <c r="L18" s="4">
         <v>7.5562347045326703</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M18" s="4">
         <v>2207.5792949868801</v>
       </c>
-      <c r="N17" s="7">
+      <c r="N18" s="4">
         <v>223.059969055794</v>
       </c>
-      <c r="O17" s="7">
+      <c r="O18" s="4">
         <v>4156.0181018469102</v>
       </c>
-      <c r="P17" s="7">
+      <c r="P18" s="4">
         <v>460.54370683425498</v>
       </c>
-      <c r="Q17" s="7">
+      <c r="Q18" s="4">
         <v>2899.76856654414</v>
       </c>
-      <c r="R17" s="7">
+      <c r="R18" s="4">
         <v>291.82410361781302</v>
       </c>
     </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B18" s="5">
+    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B19" s="2">
         <v>15</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C19" s="3">
         <v>11.397791697259001</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D19" s="4">
         <v>8.9574820403589506</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E19" s="4">
         <v>2999</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F19" s="4">
         <v>797.5</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G19" s="4">
         <v>3.4987690448760902</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H19" s="4">
         <v>3.8055366277694702</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I19" s="4">
         <v>76.525940687686301</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J19" s="4">
         <v>27.431097631238899</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K19" s="4">
         <v>5.3432587407557897</v>
       </c>
-      <c r="L18" s="7">
+      <c r="L19" s="4">
         <v>6.8589153043169198</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M19" s="4">
         <v>2188.0261028330501</v>
       </c>
-      <c r="N18" s="7">
+      <c r="N19" s="4">
         <v>230.466721028769</v>
       </c>
-      <c r="O18" s="7">
+      <c r="O19" s="4">
         <v>4170.0630165111097</v>
       </c>
-      <c r="P18" s="7">
+      <c r="P19" s="4">
         <v>461.75170750645702</v>
       </c>
-      <c r="Q18" s="7">
+      <c r="Q19" s="4">
         <v>2918.8076068509199</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R19" s="4">
         <v>298.60771100033202</v>
       </c>
     </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="5">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
         <v>20</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C20" s="3">
         <v>11.391721465492401</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D20" s="4">
         <v>8.9256532034935798</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E20" s="4">
         <v>2999</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F20" s="4">
         <v>784</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G20" s="4">
         <v>3.3839026689529401</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H20" s="4">
         <v>4.1419624090194702</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I20" s="4">
         <v>76.424121976313302</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J20" s="4">
         <v>27.670855211572899</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K20" s="4">
         <v>5.0826277639256299</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L20" s="4">
         <v>7.5324125135850304</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M20" s="4">
         <v>2165.5005571523002</v>
       </c>
-      <c r="N19" s="7">
+      <c r="N20" s="4">
         <v>228.663519397318</v>
       </c>
-      <c r="O19" s="7">
+      <c r="O20" s="4">
         <v>4150.1652158317302</v>
       </c>
-      <c r="P19" s="7">
+      <c r="P20" s="4">
         <v>455.92865647283202</v>
       </c>
-      <c r="Q19" s="7">
+      <c r="Q20" s="4">
         <v>2878.34886643348</v>
       </c>
-      <c r="R19" s="7">
+      <c r="R20" s="4">
         <v>294.88306090238001</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B20" s="5">
+    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B21" s="2">
         <v>30</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C21" s="3">
         <v>11.3895002303457</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D21" s="4">
         <v>8.9360762059904602</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E21" s="4">
         <v>2999</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F21" s="4">
         <v>791</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G21" s="4">
         <v>3.3733670711517298</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H21" s="4">
         <v>4.3774501085281301</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I21" s="4">
         <v>76.658270244210001</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J21" s="4">
         <v>27.711303926068101</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K21" s="4">
         <v>5.05863068088067</v>
       </c>
-      <c r="L20" s="7">
+      <c r="L21" s="4">
         <v>8.0374148423492908</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M21" s="4">
         <v>2155.57102761645</v>
       </c>
-      <c r="N20" s="7">
+      <c r="N21" s="4">
         <v>228.60284884533201</v>
       </c>
-      <c r="O20" s="7">
+      <c r="O21" s="4">
         <v>4146.3802391168101</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P21" s="4">
         <v>454.48558466680498</v>
       </c>
-      <c r="Q20" s="7">
+      <c r="Q21" s="4">
         <v>2859.5480720509599</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R21" s="4">
         <v>298.82287439698399</v>
       </c>
     </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="5">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B22" s="2">
         <v>40</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C22" s="3">
         <v>11.392381708597499</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D22" s="4">
         <v>8.9138742965783795</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E22" s="4">
         <v>2999</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F22" s="4">
         <v>788</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G22" s="4">
         <v>3.3590615987777701</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H22" s="4">
         <v>4.5935047864913896</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I22" s="4">
         <v>76.002385427683905</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J22" s="4">
         <v>27.675397925874499</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K22" s="4">
         <v>5.0266478270434503</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L22" s="4">
         <v>9.3723565570402805</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M22" s="4">
         <v>2185.7014851935101</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N22" s="4">
         <v>229.99388530584901</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O22" s="4">
         <v>4145.62030679088</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P22" s="4">
         <v>446.14572519702301</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q22" s="4">
         <v>2889.03739207437</v>
       </c>
-      <c r="R21" s="7">
+      <c r="R22" s="4">
         <v>295.09605379222501</v>
       </c>
     </row>
-    <row r="22" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="10">
+    <row r="23" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="7">
         <v>50</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C23" s="3">
         <v>11.3897375452937</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D23" s="4">
         <v>8.9543659195720604</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E23" s="4">
         <v>2999</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F23" s="4">
         <v>789</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G23" s="4">
         <v>3.5961606502532901</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H23" s="4">
         <v>4.4781824350357002</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I23" s="4">
         <v>76.496873641436196</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J23" s="4">
         <v>27.202809992980701</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K23" s="4">
         <v>5.5709961266328296</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L23" s="4">
         <v>8.1865092554111207</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M23" s="4">
         <v>2180.4209513359101</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N23" s="4">
         <v>228.853662203759</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O23" s="4">
         <v>4147.4114259437501</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P23" s="4">
         <v>458.93588691739899</v>
       </c>
-      <c r="Q22" s="7">
+      <c r="Q23" s="4">
         <v>2899.90522997688</v>
       </c>
-      <c r="R22" s="7">
+      <c r="R23" s="4">
         <v>295.18648961612001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:R3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>